<commit_message>
fixed a few things in example metadata files, added a bacteria fasta for Cd and then also changed a few of the test params
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE60236-467F-4349-BC3A-1FA48A969E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358840D5-BA09-3D48-A9BA-839F3C82E709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="61200" windowHeight="36420" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t>Submission info</t>
   </si>
@@ -134,9 +134,6 @@
     <t>illumina_sra_file_path_1</t>
   </si>
   <si>
-    <t>CP040557.1</t>
-  </si>
-  <si>
     <t>Homo sapiens</t>
   </si>
   <si>
@@ -173,18 +170,12 @@
     <t>2022-06</t>
   </si>
   <si>
-    <t>Michael</t>
-  </si>
-  <si>
     <t>fasta_file_name</t>
   </si>
   <si>
     <t>Cdiphtheriae</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>SRA - all</t>
   </si>
   <si>
@@ -234,6 +225,45 @@
   </si>
   <si>
     <t>test_field_3</t>
+  </si>
+  <si>
+    <t>CP040557</t>
+  </si>
+  <si>
+    <t>BX248355</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Black Bird Labs</t>
+  </si>
+  <si>
+    <t>Bio intelligence</t>
+  </si>
+  <si>
+    <t>Clinical</t>
+  </si>
+  <si>
+    <t>CP040557_Cd</t>
+  </si>
+  <si>
+    <t>BX248355_Cd</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/CP040557_test_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/CP040557_test_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/BX248355_test_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/BX248355_test_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -676,18 +706,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:AZ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
+      <selection activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="46" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -704,57 +734,57 @@
       </c>
       <c r="AD1" s="3"/>
       <c r="AE1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AW1" s="3"/>
       <c r="AX1" s="3"/>
       <c r="AY1" s="3"/>
     </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>7</v>
@@ -829,78 +859,152 @@
         <v>30</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AM2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AN2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AU2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AW2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" t="s">
         <v>43</v>
       </c>
-      <c r="AW2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX2" s="7" t="s">
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="AY2" s="7" t="s">
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
         <v>65</v>
       </c>
-      <c r="AZ2" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" t="s">
         <v>33</v>
       </c>
-      <c r="P3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="T4" t="s">
         <v>34</v>
       </c>
-      <c r="T3" t="s">
-        <v>35</v>
-      </c>
-      <c r="V3" t="s">
-        <v>48</v>
+      <c r="V4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify headers in diphtheria multifasta
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F09BAD-0740-40FD-B9E4-3BEB0DE121D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BFF1B9-905E-4DE3-99B5-AD2E145726E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>Submission info</t>
   </si>
@@ -248,12 +248,6 @@
     <t>local</t>
   </si>
   <si>
-    <t>BX248355</t>
-  </si>
-  <si>
-    <t>BX248355_Cd</t>
-  </si>
-  <si>
     <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/CP040557_R1.fastq.gz</t>
   </si>
   <si>
@@ -264,6 +258,27 @@
   </si>
   <si>
     <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/BX248355_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>BX248355.1-segment2</t>
+  </si>
+  <si>
+    <t>BX248355.1-segment3</t>
+  </si>
+  <si>
+    <t>BX248355.1-segment4</t>
+  </si>
+  <si>
+    <t>BBL-BIOINTEL</t>
+  </si>
+  <si>
+    <t>BX248355.1-segment2_Cd</t>
+  </si>
+  <si>
+    <t>BX248355.1-segment3_Cd</t>
+  </si>
+  <si>
+    <t>BX248355.1-segment4_Cd</t>
   </si>
 </sst>
 </file>
@@ -705,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:AZ4"/>
+  <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AQ12" sqref="AQ12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +962,9 @@
       <c r="B3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>64</v>
@@ -1010,10 +1027,10 @@
         <v>69</v>
       </c>
       <c r="AM3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
@@ -1030,12 +1047,14 @@
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>64</v>
@@ -1050,7 +1069,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>67</v>
@@ -1086,7 +1105,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
@@ -1098,10 +1117,10 @@
         <v>69</v>
       </c>
       <c r="AM4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
@@ -1116,6 +1135,186 @@
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
     </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change the . to - in species ID, in multifasta and metadata
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BFF1B9-905E-4DE3-99B5-AD2E145726E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3D4DE7-D062-4A64-8913-26917A9813C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
   <si>
     <t>Submission info</t>
   </si>
@@ -279,6 +279,24 @@
   </si>
   <si>
     <t>BX248355.1-segment4_Cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BX248355.1-segment2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BX248355.1-segment3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BX248355.1-segment4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BX248355-1-segment2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BX248355-1-segment3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BX248355-1-segment4 </t>
   </si>
 </sst>
 </file>
@@ -723,7 +741,7 @@
   <dimension ref="A1:AZ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,10 +1065,10 @@
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>77</v>
@@ -1137,10 +1155,10 @@
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>77</v>
@@ -1227,10 +1245,10 @@
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
upload the correct, updated metadata files
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3D4DE7-D062-4A64-8913-26917A9813C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17672ACF-645D-441E-8BAB-52DC7A95984B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
   <si>
     <t>Submission info</t>
   </si>
@@ -170,9 +170,6 @@
     <t>2022-06</t>
   </si>
   <si>
-    <t>fasta_file_name</t>
-  </si>
-  <si>
     <t>Cdiphtheriae</t>
   </si>
   <si>
@@ -248,18 +245,6 @@
     <t>local</t>
   </si>
   <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/CP040557_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/BX248355_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/CP040557_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/BX248355_R2.fastq.gz</t>
-  </si>
-  <si>
     <t>BX248355.1-segment2</t>
   </si>
   <si>
@@ -297,6 +282,27 @@
   </si>
   <si>
     <t xml:space="preserve">BX248355-1-segment4 </t>
+  </si>
+  <si>
+    <t>fasta_path</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/Cdiphtheriae/CP040557.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/Cdiphtheriae/BX248355.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/Cdiphtheriae/CP040557_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/Cdiphtheriae/BX248355_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/Cdiphtheriae/CP040557_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/Cdiphtheriae/BX248355_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -740,13 +746,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
   <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AN6" sqref="AN6:AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="46" width="24" customWidth="1"/>
+    <col min="1" max="47" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -788,13 +794,13 @@
       </c>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
@@ -802,10 +808,10 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
@@ -822,40 +828,40 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>7</v>
@@ -908,99 +914,99 @@
       <c r="AD2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AE2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="AY2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1008,7 +1014,7 @@
         <v>32</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>43</v>
@@ -1033,24 +1039,26 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF3" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
-      <c r="AL3" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="AL3" s="1"/>
       <c r="AM3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO3" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
@@ -1065,32 +1073,32 @@
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1098,7 +1106,7 @@
         <v>32</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>43</v>
@@ -1123,24 +1131,26 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF4" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
-      <c r="AL4" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="AL4" s="1"/>
       <c r="AM4" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO4" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
@@ -1155,32 +1165,32 @@
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1188,7 +1198,7 @@
         <v>32</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>43</v>
@@ -1213,24 +1223,26 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF5" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
-      <c r="AL5" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="AL5" s="1"/>
       <c r="AM5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO5" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
@@ -1245,32 +1257,32 @@
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -1278,7 +1290,7 @@
         <v>32</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>43</v>
@@ -1303,24 +1315,26 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF6" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
-      <c r="AL6" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="AL6" s="1"/>
       <c r="AM6" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO6" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>

</xml_diff>

<commit_message>
remove spaces from metadata (quick fix, will do in code later)
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17672ACF-645D-441E-8BAB-52DC7A95984B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA441B6-1362-4084-A9C9-90293623D6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
@@ -275,12 +275,6 @@
     <t xml:space="preserve">BX248355.1-segment4 </t>
   </si>
   <si>
-    <t xml:space="preserve">BX248355-1-segment2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BX248355-1-segment3 </t>
-  </si>
-  <si>
     <t xml:space="preserve">BX248355-1-segment4 </t>
   </si>
   <si>
@@ -303,6 +297,12 @@
   </si>
   <si>
     <t>assets/sample_fastqs/Cdiphtheriae/BX248355_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>BX248355-1-segment3</t>
+  </si>
+  <si>
+    <t>BX248355-1-segment2</t>
   </si>
 </sst>
 </file>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
   <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AN6" sqref="AN6:AO6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +915,7 @@
         <v>23</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>24</v>
@@ -1039,7 +1039,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>67</v>
@@ -1054,10 +1054,10 @@
         <v>68</v>
       </c>
       <c r="AN3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>76</v>
@@ -1131,7 +1131,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AF4" s="1" t="s">
         <v>73</v>
@@ -1146,10 +1146,10 @@
         <v>68</v>
       </c>
       <c r="AN4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO4" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>77</v>
@@ -1223,7 +1223,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AF5" s="1" t="s">
         <v>74</v>
@@ -1238,10 +1238,10 @@
         <v>68</v>
       </c>
       <c r="AN5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO5" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>78</v>
@@ -1315,7 +1315,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>75</v>
@@ -1330,10 +1330,10 @@
         <v>68</v>
       </c>
       <c r="AN6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO6" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>

</xml_diff>

<commit_message>
fixed typo in test metadata
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA441B6-1362-4084-A9C9-90293623D6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C641C-80EE-DC46-87CA-8EB7418499F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -275,9 +275,6 @@
     <t xml:space="preserve">BX248355.1-segment4 </t>
   </si>
   <si>
-    <t xml:space="preserve">BX248355-1-segment4 </t>
-  </si>
-  <si>
     <t>fasta_path</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>BX248355-1-segment2</t>
+  </si>
+  <si>
+    <t>BX248355-1-segment4</t>
   </si>
 </sst>
 </file>
@@ -448,9 +448,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -488,7 +488,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -594,7 +594,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -736,7 +736,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -747,15 +747,15 @@
   <dimension ref="A1:AZ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="47" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,7 +823,7 @@
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
     </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -915,7 +915,7 @@
         <v>23</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>24</v>
@@ -979,7 +979,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>67</v>
@@ -1054,10 +1054,10 @@
         <v>68</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
@@ -1071,9 +1071,9 @@
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>76</v>
@@ -1131,7 +1131,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AF4" s="1" t="s">
         <v>73</v>
@@ -1146,10 +1146,10 @@
         <v>68</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
@@ -1163,9 +1163,9 @@
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>77</v>
@@ -1223,7 +1223,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AF5" s="1" t="s">
         <v>74</v>
@@ -1238,10 +1238,10 @@
         <v>68</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
@@ -1255,9 +1255,9 @@
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>78</v>
@@ -1315,7 +1315,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>75</v>
@@ -1330,10 +1330,10 @@
         <v>68</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>

</xml_diff>

<commit_message>
remove the .1 from BS248355.1 in the BX248355.fasta headers and metadata
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C641C-80EE-DC46-87CA-8EB7418499F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F0DB9-D91D-4C1B-A1B8-ECFB378A45F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="5325" yWindow="2250" windowWidth="21600" windowHeight="11265" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Submission info</t>
   </si>
@@ -245,36 +245,9 @@
     <t>local</t>
   </si>
   <si>
-    <t>BX248355.1-segment2</t>
-  </si>
-  <si>
-    <t>BX248355.1-segment3</t>
-  </si>
-  <si>
-    <t>BX248355.1-segment4</t>
-  </si>
-  <si>
     <t>BBL-BIOINTEL</t>
   </si>
   <si>
-    <t>BX248355.1-segment2_Cd</t>
-  </si>
-  <si>
-    <t>BX248355.1-segment3_Cd</t>
-  </si>
-  <si>
-    <t>BX248355.1-segment4_Cd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BX248355.1-segment2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BX248355.1-segment3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BX248355.1-segment4 </t>
-  </si>
-  <si>
     <t>fasta_path</t>
   </si>
   <si>
@@ -296,13 +269,10 @@
     <t>assets/sample_fastqs/Cdiphtheriae/BX248355_R2.fastq.gz</t>
   </si>
   <si>
-    <t>BX248355-1-segment3</t>
-  </si>
-  <si>
-    <t>BX248355-1-segment2</t>
-  </si>
-  <si>
-    <t>BX248355-1-segment4</t>
+    <t>BX248355.1</t>
+  </si>
+  <si>
+    <t>BX248355</t>
   </si>
 </sst>
 </file>
@@ -448,9 +418,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -488,7 +458,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -594,7 +564,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -736,7 +706,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -744,18 +714,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:AZ6"/>
+  <dimension ref="A1:AZ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="47" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,7 +793,7 @@
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
     </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -915,7 +885,7 @@
         <v>23</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>24</v>
@@ -979,7 +949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -987,7 +957,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
@@ -1039,7 +1009,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>67</v>
@@ -1054,10 +1024,10 @@
         <v>68</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
@@ -1071,15 +1041,15 @@
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
@@ -1095,7 +1065,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>66</v>
@@ -1131,10 +1101,10 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
@@ -1146,10 +1116,10 @@
         <v>68</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
@@ -1163,190 +1133,6 @@
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AP5" s="1"/>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1"/>
-      <c r="AT5" s="1"/>
-      <c r="AU5" s="1"/>
-      <c r="AV5" s="1"/>
-      <c r="AW5" s="1"/>
-      <c r="AX5" s="1"/>
-      <c r="AY5" s="1"/>
-      <c r="AZ5" s="1"/>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
-      <c r="AT6" s="1"/>
-      <c r="AU6" s="1"/>
-      <c r="AV6" s="1"/>
-      <c r="AW6" s="1"/>
-      <c r="AX6" s="1"/>
-      <c r="AY6" s="1"/>
-      <c r="AZ6" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>